<commit_message>
Removed spaces in excel sheet.
</commit_message>
<xml_diff>
--- a/word_pairs/Icelandic-English-Danish_40Words.xlsx
+++ b/word_pairs/Icelandic-English-Danish_40Words.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Emily_DTU_BA5\EPFL\BA5\02455_ExpCognitiveScience\CognitiveExperiment\word_pairs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFB7E078-03FF-4BF0-AB39-85CB729C880F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93F161F2-5A3F-42E1-9F86-4A489465E648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
   <si>
     <t>Icelandic</t>
   </si>
@@ -366,34 +366,31 @@
     <t>humør</t>
   </si>
   <si>
-    <t xml:space="preserve">museum </t>
-  </si>
-  <si>
     <t>museum</t>
   </si>
   <si>
-    <t xml:space="preserve">trip </t>
-  </si>
-  <si>
-    <t xml:space="preserve">tur </t>
-  </si>
-  <si>
-    <t xml:space="preserve">mood </t>
-  </si>
-  <si>
     <t>success</t>
   </si>
   <si>
-    <t xml:space="preserve">succes </t>
-  </si>
-  <si>
-    <t xml:space="preserve">project </t>
-  </si>
-  <si>
-    <t xml:space="preserve">number </t>
-  </si>
-  <si>
     <t>antal</t>
+  </si>
+  <si>
+    <t>trip</t>
+  </si>
+  <si>
+    <t>project</t>
+  </si>
+  <si>
+    <t>mood</t>
+  </si>
+  <si>
+    <t>number</t>
+  </si>
+  <si>
+    <t>tur</t>
+  </si>
+  <si>
+    <t>succes</t>
   </si>
 </sst>
 </file>
@@ -727,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="127" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1096,7 +1093,7 @@
         <v>113</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1104,10 +1101,10 @@
         <v>97</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1148,10 +1145,10 @@
         <v>107</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1159,7 +1156,7 @@
         <v>108</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>109</v>
@@ -1170,10 +1167,10 @@
         <v>110</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1181,7 +1178,7 @@
         <v>111</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>112</v>

</xml_diff>